<commit_message>
Actualizar datos del documento de empleado.xlsx
</commit_message>
<xml_diff>
--- a/Espressoft-master/documentos_excel/empleados/empleado.xlsx
+++ b/Espressoft-master/documentos_excel/empleados/empleado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNISON\2023-1\Practicas de desarrollo de sistemas\Espressoft\Espressoft-master\documentos_excel\empleados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BB0066-0CEE-4A44-AF7D-910D94698A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84311934-D0E2-471E-8A31-523E77663AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="5715" windowWidth="20730" windowHeight="11160" xr2:uid="{60B3716A-2365-46CF-B740-82791724B4B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60B3716A-2365-46CF-B740-82791724B4B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
   <si>
     <t>tipo_empleado</t>
   </si>
@@ -59,9 +59,6 @@
     <t>correo</t>
   </si>
   <si>
-    <t>123_admi</t>
-  </si>
-  <si>
     <t>Luis</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
   </si>
   <si>
     <t>LuisQuintanaH@gmail.com</t>
-  </si>
-  <si>
-    <t>123_gere</t>
   </si>
   <si>
     <t>Fatima</t>
@@ -652,7 +646,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,13 +663,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -701,19 +695,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="1">
+        <v>123</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -722,7 +716,7 @@
         <v>6621989026</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -730,19 +724,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="1">
+        <v>123</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -751,7 +745,7 @@
         <v>6622978568</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -759,19 +753,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -780,7 +774,7 @@
         <v>6621681862</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -788,19 +782,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -809,7 +803,7 @@
         <v>6623484023</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -817,19 +811,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -838,7 +832,7 @@
         <v>6623203133</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -846,19 +840,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -867,7 +861,7 @@
         <v>6623486765</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -875,19 +869,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -896,7 +890,7 @@
         <v>6621526659</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -904,19 +898,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
@@ -925,7 +919,7 @@
         <v>6624158571</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -933,19 +927,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -954,7 +948,7 @@
         <v>6625837497</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -962,19 +956,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -983,7 +977,7 @@
         <v>6621571596</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -991,19 +985,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -1012,7 +1006,7 @@
         <v>6624183933</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1020,19 +1014,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -1041,7 +1035,7 @@
         <v>6621982383</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1049,19 +1043,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="G14" s="1">
         <v>1</v>
@@ -1070,7 +1064,7 @@
         <v>6624778624</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1078,19 +1072,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
@@ -1099,7 +1093,7 @@
         <v>6623266998</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1136,6 +1130,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6987639e-b33b-4be7-98ef-a8e69327d5ad" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100608EF00C4280014084C922EEA59EF04F" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b987c191771a38deb8ec0017aadcc3e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6987639e-b33b-4be7-98ef-a8e69327d5ad" xmlns:ns4="e86b59b6-c75e-4fee-8b44-5e665f30d7e5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fbebdc5b109fa6c27bed846c0a30e487" ns3:_="" ns4:_="">
     <xsd:import namespace="6987639e-b33b-4be7-98ef-a8e69327d5ad"/>
@@ -1370,24 +1381,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7C95158-D69B-473E-A372-BD47BA78F692}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6987639e-b33b-4be7-98ef-a8e69327d5ad"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6987639e-b33b-4be7-98ef-a8e69327d5ad" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{972A6D9D-0D27-4CD6-8237-8560B3DDDE60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8B9500-63A7-4F51-87EF-7AABD93CF179}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1404,22 +1416,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{972A6D9D-0D27-4CD6-8237-8560B3DDDE60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7C95158-D69B-473E-A372-BD47BA78F692}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6987639e-b33b-4be7-98ef-a8e69327d5ad"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>